<commit_message>
Fix: added missing argument metrics_dic_d2d in bs2d_ul_outputs() call
</commit_message>
<xml_diff>
--- a/simulation_settings/bs_parameters.xlsx
+++ b/simulation_settings/bs_parameters.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -594,75 +594,6 @@
       </c>
       <c r="S2" t="inlineStr"/>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>39.2337738</v>
-      </c>
-      <c r="C3" t="n">
-        <v>9.12153844</v>
-      </c>
-      <c r="D3" t="n">
-        <v>50000</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>sat</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>HAPS</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Sat_ax</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>dual</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>C_ntn</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>A_ntn</t>
-        </is>
-      </c>
-      <c r="K3" t="n">
-        <v>2</v>
-      </c>
-      <c r="L3" t="n">
-        <v>2</v>
-      </c>
-      <c r="M3" t="n">
-        <v>50</v>
-      </c>
-      <c r="N3" t="n">
-        <v>36</v>
-      </c>
-      <c r="O3" t="n">
-        <v>30</v>
-      </c>
-      <c r="P3" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>7</v>
-      </c>
-      <c r="R3" t="inlineStr"/>
-      <c r="S3" t="n">
-        <v>85</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>